<commit_message>
Solved Config on displays
File added ssf config, has all the display configurations
</commit_message>
<xml_diff>
--- a/platform_db_list.xlsx
+++ b/platform_db_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PLATFORMDB" sheetId="1" r:id="rId1"/>
@@ -1979,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11952,9 +11952,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12589,7 +12589,7 @@
         <v>424</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>425</v>
+        <v>24</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>408</v>
@@ -12618,7 +12618,7 @@
         <v>424</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>425</v>
+        <v>24</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>408</v>
@@ -12647,7 +12647,7 @@
         <v>424</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>425</v>
+        <v>24</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>408</v>
@@ -12676,7 +12676,7 @@
         <v>424</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>425</v>
+        <v>24</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>408</v>
@@ -12705,7 +12705,7 @@
         <v>424</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>425</v>
+        <v>24</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>408</v>
@@ -12734,7 +12734,7 @@
         <v>424</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>425</v>
+        <v>24</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>408</v>

</xml_diff>